<commit_message>
<Fix> Fixed bugs in the ‘Nearby’ module, improved the structure of items, enabled correct interactions with items and containers, streamlined interface responsibilities, fixed display errors during interactions, and added a few test assets.
</commit_message>
<xml_diff>
--- a/Assets/Configs/Inventory/Property/Xlsxs/DurablePropertyData.xlsx
+++ b/Assets/Configs/Inventory/Property/Xlsxs/DurablePropertyData.xlsx
@@ -49,7 +49,7 @@
     <t>铁斧头</t>
   </si>
   <si>
-    <t>和金斧头</t>
+    <t>合金斧头</t>
   </si>
 </sst>
 </file>
@@ -62,13 +62,19 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="HarmonyOS Sans SC"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -535,141 +541,147 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -986,75 +998,76 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.2636363636364" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="13.2636363636364" defaultRowHeight="15.5" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="13.2636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18.1727272727273" customWidth="1"/>
-    <col min="4" max="16384" width="13.2636363636364" customWidth="1"/>
+    <col min="1" max="1" width="8.21818181818182" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.2636363636364" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1727272727273" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="13.2636363636364" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>10011</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>100</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>10012</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>110</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>10013</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>120</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>10014</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>130</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>